<commit_message>
PRJ to remove from .git
</commit_message>
<xml_diff>
--- a/PRJ/Work2024.xlsx
+++ b/PRJ/Work2024.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4440" yWindow="3510" windowWidth="20910" windowHeight="11775" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lavori" sheetId="1" state="visible" r:id="rId1"/>
@@ -61,6 +61,14 @@
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -131,6 +139,28 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabella1" displayName="Tabella1" ref="A1:I4" headerRowCount="1" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:I4"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Azienda"/>
+    <tableColumn id="2" name="Cliente"/>
+    <tableColumn id="3" name="Nome scheda"/>
+    <tableColumn id="4" name="Ore Preventivo"/>
+    <tableColumn id="5" name="Prezzo unitario"/>
+    <tableColumn id="6" name="Preventivo">
+      <calculatedColumnFormula>D2*E2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" name="Preventivo no rivalsa" dataDxfId="0">
+      <calculatedColumnFormula>D2*data!J7</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" name="Ore lavorate"/>
+    <tableColumn id="9" name="Stato"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -429,155 +459,198 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A4:I6"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.28515625" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="13.42578125" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="14.42578125" customWidth="1" min="4" max="4"/>
-    <col width="14.42578125" customWidth="1" min="7" max="7"/>
-    <col width="8.28515625" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="9.5703125" customWidth="1" min="2" max="2"/>
+    <col width="15.140625" customWidth="1" min="3" max="3"/>
+    <col width="16.5703125" customWidth="1" min="4" max="4"/>
+    <col width="16.42578125" customWidth="1" min="5" max="5"/>
+    <col width="12.85546875" customWidth="1" min="6" max="6"/>
+    <col width="21.7109375" customWidth="1" min="7" max="7"/>
+    <col width="14.140625" customWidth="1" min="8" max="8"/>
     <col width="13.5703125" bestFit="1" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
-    <row r="4" ht="45" customHeight="1">
+    <row r="1" ht="45" customHeight="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Azienda</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Cliente</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Nome scheda</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Ore Preventivo</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Prezzo unitario</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Preventivo</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Preventivo no rivalsa</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Ore lavorate</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Stato</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Telma</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ESTE</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>FEEM v1</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>34</v>
+      </c>
+      <c r="E2" t="n">
+        <v>31</v>
+      </c>
+      <c r="F2">
+        <f>D2*E2</f>
+        <v/>
+      </c>
+      <c r="G2" s="2">
+        <f>D2*data!J14</f>
+        <v/>
+      </c>
+      <c r="H2" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>In lavorazione</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Telma</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Robomagister</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ELC23</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>34</v>
+      </c>
+      <c r="E3" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="F3">
+        <f>D3*E3</f>
+        <v/>
+      </c>
+      <c r="G3" s="2">
+        <f>D3*data!J8</f>
+        <v/>
+      </c>
+      <c r="H3" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>In lavorazione</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Azienda</t>
+          <t>Telma</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cliente</t>
+          <t>TEST</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Nome scheda</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="inlineStr">
-        <is>
-          <t>Ore Preventivo</t>
-        </is>
-      </c>
-      <c r="E4" s="1" t="inlineStr">
-        <is>
-          <t>Prezzo unitario</t>
-        </is>
-      </c>
-      <c r="F4" s="1" t="inlineStr">
-        <is>
-          <t>Preventivo</t>
-        </is>
-      </c>
-      <c r="G4" s="1" t="inlineStr">
-        <is>
-          <t>Preventivo no rivalsa</t>
-        </is>
-      </c>
-      <c r="H4" s="1" t="inlineStr">
-        <is>
-          <t>Ore lavorate</t>
-        </is>
-      </c>
-      <c r="I4" s="1" t="inlineStr">
-        <is>
-          <t>Stato</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Telma</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>ESTE</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>FEEM v1</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>34</v>
-      </c>
-      <c r="E5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F5">
-        <f>D5*E5</f>
-        <v/>
-      </c>
-      <c r="G5" s="2">
-        <f>D5*data!J14</f>
-        <v/>
-      </c>
-      <c r="H5" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>In lavorazione</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Telma</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Robomagister</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>ELC23</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>34</v>
-      </c>
-      <c r="E6" t="n">
-        <v>27.5</v>
-      </c>
-      <c r="F6">
-        <f>D6*E6</f>
-        <v/>
-      </c>
-      <c r="G6" s="2">
-        <f>D6*data!J8</f>
-        <v/>
-      </c>
-      <c r="H6" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>In lavorazione</t>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Inviato</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -590,7 +663,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
# TBD Minutes are displayed without 0 --> fixed # TBD review prj update --> seems ok # TBD config ini configurable with interface (insert settings button)  --> Done interface # TBD Force edit before update timer  ---> button for edit start timer # TBD handle errors when is project running and are added some lines in excel --> 18/12/2023 no errors found # TBD Column name in table --> added column name in config.ini # TBD better graphics!! --> some improvements made # TBD Verify round function on timestep and how to update the timer or force it
</commit_message>
<xml_diff>
--- a/PRJ/Work2024.xlsx
+++ b/PRJ/Work2024.xlsx
@@ -3,11 +3,12 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4440" yWindow="3510" windowWidth="20910" windowHeight="11775" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lavori" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="data" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Testdata" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="CostoOrario">data!$C$1</definedName>
@@ -466,7 +467,7 @@
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -561,7 +562,7 @@
         <v/>
       </c>
       <c r="H2" t="n">
-        <v>9.5</v>
+        <v>9.25</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -600,7 +601,7 @@
         <v/>
       </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>15.75</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -797,4 +798,37 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>In lavorazione</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Fatturabile</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>